<commit_message>
sesion 11, implementacion de Allure reporting
</commit_message>
<xml_diff>
--- a/selenium-java/selenium-java/src/test/resources/testdata/clientes-data.xlsx
+++ b/selenium-java/selenium-java/src/test/resources/testdata/clientes-data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="593">
   <si>
     <t>CHOPS</t>
   </si>
@@ -136,9 +136,6 @@
     <t>40.67.89.89</t>
   </si>
   <si>
-    <t>EASTC</t>
-  </si>
-  <si>
     <t>Eastern Connection</t>
   </si>
   <si>
@@ -1787,6 +1784,15 @@
   </si>
   <si>
     <t>01307</t>
+  </si>
+  <si>
+    <t>Accounting Managers</t>
+  </si>
+  <si>
+    <t>🇲🇽 Mexicos</t>
+  </si>
+  <si>
+    <t>EASTCs</t>
   </si>
 </sst>
 </file>
@@ -2131,8 +2137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="F83" sqref="F83"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2150,37 +2156,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B1" t="s">
         <v>157</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>158</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>159</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>434</v>
+      </c>
+      <c r="F1" t="s">
+        <v>435</v>
+      </c>
+      <c r="G1" t="s">
         <v>160</v>
       </c>
-      <c r="E1" t="s">
-        <v>435</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I1" t="s">
         <v>436</v>
       </c>
-      <c r="G1" t="s">
-        <v>161</v>
-      </c>
-      <c r="H1" t="s">
-        <v>162</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>437</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>438</v>
-      </c>
-      <c r="K1" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -2191,7 +2197,7 @@
         <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D2" t="s">
         <v>30</v>
@@ -2200,7 +2206,7 @@
         <v>52066</v>
       </c>
       <c r="G2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H2" t="s">
         <v>31</v>
@@ -2229,7 +2235,7 @@
         <v>44000</v>
       </c>
       <c r="G3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H3" t="s">
         <v>37</v>
@@ -2243,118 +2249,118 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>592</v>
+      </c>
+      <c r="B4" t="s">
         <v>40</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>41</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>42</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>43</v>
       </c>
-      <c r="F4" t="s">
-        <v>44</v>
-      </c>
       <c r="G4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H4" t="s">
         <v>19</v>
       </c>
       <c r="I4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" t="s">
         <v>45</v>
-      </c>
-      <c r="J4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" t="s">
         <v>47</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>48</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>49</v>
-      </c>
-      <c r="D5" t="s">
-        <v>50</v>
       </c>
       <c r="F5">
         <v>8010</v>
       </c>
       <c r="G5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" t="s">
         <v>51</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>52</v>
-      </c>
-      <c r="J5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
         <v>54</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>55</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>56</v>
-      </c>
-      <c r="D6" t="s">
-        <v>57</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G6" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H6" t="s">
         <v>12</v>
       </c>
       <c r="I6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" t="s">
         <v>60</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>61</v>
       </c>
-      <c r="C7" t="s">
-        <v>62</v>
-      </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>590</v>
       </c>
       <c r="F7">
         <v>28034</v>
       </c>
       <c r="G7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" t="s">
         <v>64</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>65</v>
-      </c>
-      <c r="J7" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -2374,7 +2380,7 @@
         <v>70563</v>
       </c>
       <c r="G8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H8" t="s">
         <v>25</v>
@@ -2388,97 +2394,97 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" t="s">
         <v>67</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>68</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>69</v>
-      </c>
-      <c r="D9" t="s">
-        <v>70</v>
       </c>
       <c r="F9">
         <v>59000</v>
       </c>
       <c r="G9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9" t="s">
         <v>71</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>72</v>
-      </c>
-      <c r="J9" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" t="s">
         <v>74</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>75</v>
-      </c>
-      <c r="C10" t="s">
-        <v>76</v>
       </c>
       <c r="D10" t="s">
         <v>3</v>
       </c>
       <c r="F10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" t="s">
+        <v>165</v>
+      </c>
+      <c r="H10" t="s">
         <v>77</v>
       </c>
-      <c r="G10" t="s">
-        <v>166</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>78</v>
-      </c>
-      <c r="I10" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>263</v>
+      </c>
+      <c r="B11" t="s">
         <v>264</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>265</v>
       </c>
-      <c r="C11" t="s">
-        <v>266</v>
-      </c>
       <c r="D11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F11">
         <v>44000</v>
       </c>
       <c r="G11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H11" t="s">
         <v>37</v>
       </c>
       <c r="I11" t="s">
+        <v>439</v>
+      </c>
+      <c r="J11" t="s">
         <v>440</v>
-      </c>
-      <c r="J11" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>266</v>
+      </c>
+      <c r="B12" t="s">
         <v>267</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>268</v>
-      </c>
-      <c r="C12" t="s">
-        <v>269</v>
       </c>
       <c r="D12" t="s">
         <v>17</v>
@@ -2487,140 +2493,140 @@
         <v>10100</v>
       </c>
       <c r="G12" t="s">
+        <v>269</v>
+      </c>
+      <c r="H12" t="s">
         <v>270</v>
       </c>
-      <c r="H12" t="s">
-        <v>271</v>
-      </c>
       <c r="I12" t="s">
+        <v>441</v>
+      </c>
+      <c r="J12" t="s">
         <v>442</v>
-      </c>
-      <c r="J12" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>271</v>
+      </c>
+      <c r="B13" t="s">
         <v>272</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>273</v>
       </c>
-      <c r="C13" t="s">
-        <v>274</v>
-      </c>
       <c r="D13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F13">
         <v>80805</v>
       </c>
       <c r="G13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H13" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="I13" t="s">
+        <v>443</v>
+      </c>
+      <c r="J13" t="s">
         <v>444</v>
-      </c>
-      <c r="J13" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>275</v>
+      </c>
+      <c r="B14" t="s">
         <v>276</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>277</v>
       </c>
-      <c r="C14" t="s">
-        <v>278</v>
-      </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F14">
         <v>1675</v>
       </c>
       <c r="G14" t="s">
+        <v>278</v>
+      </c>
+      <c r="H14" t="s">
         <v>279</v>
       </c>
-      <c r="H14" t="s">
-        <v>280</v>
-      </c>
       <c r="I14" t="s">
+        <v>445</v>
+      </c>
+      <c r="J14" t="s">
         <v>446</v>
-      </c>
-      <c r="J14" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>280</v>
+      </c>
+      <c r="B15" t="s">
         <v>281</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>282</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
+        <v>117</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>583</v>
+      </c>
+      <c r="G15" t="s">
+        <v>167</v>
+      </c>
+      <c r="H15" t="s">
         <v>283</v>
       </c>
-      <c r="D15" t="s">
-        <v>118</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>584</v>
-      </c>
-      <c r="G15" t="s">
-        <v>168</v>
-      </c>
-      <c r="H15" t="s">
-        <v>284</v>
-      </c>
       <c r="I15" t="s">
+        <v>447</v>
+      </c>
+      <c r="J15" t="s">
         <v>448</v>
-      </c>
-      <c r="J15" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>284</v>
+      </c>
+      <c r="B16" t="s">
         <v>285</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>286</v>
       </c>
-      <c r="C16" t="s">
-        <v>287</v>
-      </c>
       <c r="D16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F16">
         <v>41101</v>
       </c>
       <c r="G16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H16" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I16" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" t="s">
         <v>80</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>81</v>
-      </c>
-      <c r="C17" t="s">
-        <v>82</v>
       </c>
       <c r="D17" t="s">
         <v>17</v>
@@ -2629,140 +2635,140 @@
         <v>12209</v>
       </c>
       <c r="G17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H17" t="s">
+        <v>82</v>
+      </c>
+      <c r="I17" t="s">
         <v>83</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>84</v>
-      </c>
-      <c r="J17" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" t="s">
         <v>86</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>87</v>
-      </c>
-      <c r="C18" t="s">
-        <v>88</v>
       </c>
       <c r="D18" t="s">
         <v>3</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="G18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H18" t="s">
+        <v>88</v>
+      </c>
+      <c r="I18" t="s">
         <v>89</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>90</v>
-      </c>
-      <c r="J18" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" t="s">
         <v>92</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>93</v>
-      </c>
-      <c r="C19" t="s">
-        <v>94</v>
       </c>
       <c r="D19" t="s">
         <v>3</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="G19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" t="s">
         <v>96</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>97</v>
-      </c>
-      <c r="C20" t="s">
-        <v>98</v>
       </c>
       <c r="D20" t="s">
         <v>17</v>
       </c>
       <c r="F20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G20" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H20" t="s">
         <v>19</v>
       </c>
       <c r="I20" t="s">
+        <v>99</v>
+      </c>
+      <c r="J20" t="s">
         <v>100</v>
-      </c>
-      <c r="J20" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" t="s">
         <v>102</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>103</v>
-      </c>
-      <c r="C21" t="s">
-        <v>104</v>
       </c>
       <c r="D21" t="s">
         <v>30</v>
       </c>
       <c r="F21" t="s">
+        <v>104</v>
+      </c>
+      <c r="G21" t="s">
+        <v>165</v>
+      </c>
+      <c r="H21" t="s">
         <v>105</v>
       </c>
-      <c r="G21" t="s">
-        <v>166</v>
-      </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>106</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>107</v>
-      </c>
-      <c r="J21" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>108</v>
+      </c>
+      <c r="B22" t="s">
         <v>109</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>110</v>
-      </c>
-      <c r="C22" t="s">
-        <v>111</v>
       </c>
       <c r="D22" t="s">
         <v>17</v>
@@ -2771,56 +2777,56 @@
         <v>68306</v>
       </c>
       <c r="G22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H22" t="s">
+        <v>111</v>
+      </c>
+      <c r="I22" t="s">
         <v>112</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>113</v>
-      </c>
-      <c r="J22" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" t="s">
         <v>115</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>116</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>117</v>
-      </c>
-      <c r="D23" t="s">
-        <v>118</v>
       </c>
       <c r="F23">
         <v>67000</v>
       </c>
       <c r="G23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H23" t="s">
+        <v>118</v>
+      </c>
+      <c r="I23" t="s">
         <v>119</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>120</v>
-      </c>
-      <c r="J23" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>121</v>
+      </c>
+      <c r="B24" t="s">
         <v>122</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>123</v>
-      </c>
-      <c r="C24" t="s">
-        <v>124</v>
       </c>
       <c r="D24" t="s">
         <v>3</v>
@@ -2829,27 +2835,27 @@
         <v>28023</v>
       </c>
       <c r="G24" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I24" t="s">
+        <v>124</v>
+      </c>
+      <c r="J24" t="s">
         <v>125</v>
-      </c>
-      <c r="J24" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>126</v>
+      </c>
+      <c r="B25" t="s">
         <v>127</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>128</v>
-      </c>
-      <c r="C25" t="s">
-        <v>129</v>
       </c>
       <c r="D25" t="s">
         <v>3</v>
@@ -2858,132 +2864,132 @@
         <v>13008</v>
       </c>
       <c r="G25" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H25" t="s">
+        <v>129</v>
+      </c>
+      <c r="I25" t="s">
         <v>130</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>131</v>
-      </c>
-      <c r="J25" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>132</v>
+      </c>
+      <c r="B26" t="s">
         <v>133</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>134</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" t="s">
         <v>135</v>
       </c>
-      <c r="D26" t="s">
-        <v>63</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>136</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
+        <v>171</v>
+      </c>
+      <c r="H26" t="s">
         <v>137</v>
       </c>
-      <c r="G26" t="s">
-        <v>172</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>138</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>139</v>
-      </c>
-      <c r="J26" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>140</v>
+      </c>
+      <c r="B27" t="s">
         <v>141</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>142</v>
-      </c>
-      <c r="C27" t="s">
-        <v>143</v>
       </c>
       <c r="D27" t="s">
         <v>17</v>
       </c>
       <c r="F27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G27" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H27" t="s">
         <v>19</v>
       </c>
       <c r="I27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>145</v>
+      </c>
+      <c r="B28" t="s">
         <v>146</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>147</v>
       </c>
-      <c r="C28" t="s">
-        <v>148</v>
-      </c>
       <c r="D28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F28">
         <v>1010</v>
       </c>
       <c r="G28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H28" t="s">
+        <v>148</v>
+      </c>
+      <c r="I28" t="s">
         <v>149</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>150</v>
-      </c>
-      <c r="J28" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>151</v>
+      </c>
+      <c r="B29" t="s">
         <v>152</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>153</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="G29" t="s">
+        <v>591</v>
+      </c>
+      <c r="H29" t="s">
+        <v>88</v>
+      </c>
+      <c r="I29" t="s">
         <v>154</v>
       </c>
-      <c r="D29" t="s">
-        <v>118</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>587</v>
-      </c>
-      <c r="G29" t="s">
-        <v>164</v>
-      </c>
-      <c r="H29" t="s">
-        <v>89</v>
-      </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>155</v>
-      </c>
-      <c r="J29" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -3003,7 +3009,7 @@
         <v>3012</v>
       </c>
       <c r="G30" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H30" t="s">
         <v>4</v>
@@ -3032,7 +3038,7 @@
         <v>11</v>
       </c>
       <c r="G31" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H31" t="s">
         <v>12</v>
@@ -3058,7 +3064,7 @@
         <v>18</v>
       </c>
       <c r="G32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H32" t="s">
         <v>19</v>
@@ -3072,13 +3078,13 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>288</v>
+      </c>
+      <c r="B33" t="s">
         <v>289</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>290</v>
-      </c>
-      <c r="C33" t="s">
-        <v>291</v>
       </c>
       <c r="D33" t="s">
         <v>9</v>
@@ -3087,242 +3093,242 @@
         <v>10</v>
       </c>
       <c r="F33" t="s">
+        <v>450</v>
+      </c>
+      <c r="G33" t="s">
+        <v>170</v>
+      </c>
+      <c r="H33" t="s">
+        <v>291</v>
+      </c>
+      <c r="I33" t="s">
         <v>451</v>
-      </c>
-      <c r="G33" t="s">
-        <v>171</v>
-      </c>
-      <c r="H33" t="s">
-        <v>292</v>
-      </c>
-      <c r="I33" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>292</v>
+      </c>
+      <c r="B34" t="s">
         <v>293</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>294</v>
       </c>
-      <c r="C34" t="s">
-        <v>295</v>
-      </c>
       <c r="D34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E34" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F34">
         <v>97403</v>
       </c>
       <c r="G34" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H34" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I34" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>296</v>
+      </c>
+      <c r="B35" t="s">
         <v>297</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>298</v>
-      </c>
-      <c r="C35" t="s">
-        <v>299</v>
       </c>
       <c r="D35" t="s">
         <v>3</v>
       </c>
       <c r="E35" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F35">
         <v>1081</v>
       </c>
       <c r="G35" t="s">
+        <v>299</v>
+      </c>
+      <c r="H35" t="s">
         <v>300</v>
       </c>
-      <c r="H35" t="s">
-        <v>301</v>
-      </c>
       <c r="I35" t="s">
+        <v>455</v>
+      </c>
+      <c r="J35" t="s">
         <v>456</v>
-      </c>
-      <c r="J35" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>301</v>
+      </c>
+      <c r="B36" t="s">
         <v>302</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>303</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
+        <v>62</v>
+      </c>
+      <c r="E36" t="s">
+        <v>457</v>
+      </c>
+      <c r="F36" t="s">
+        <v>458</v>
+      </c>
+      <c r="G36" t="s">
+        <v>170</v>
+      </c>
+      <c r="H36" t="s">
         <v>304</v>
       </c>
-      <c r="D36" t="s">
-        <v>63</v>
-      </c>
-      <c r="E36" t="s">
-        <v>458</v>
-      </c>
-      <c r="F36" t="s">
+      <c r="I36" t="s">
         <v>459</v>
       </c>
-      <c r="G36" t="s">
-        <v>171</v>
-      </c>
-      <c r="H36" t="s">
-        <v>305</v>
-      </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>460</v>
-      </c>
-      <c r="J36" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>305</v>
+      </c>
+      <c r="B37" t="s">
         <v>306</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>307</v>
-      </c>
-      <c r="C37" t="s">
-        <v>308</v>
       </c>
       <c r="D37" t="s">
         <v>17</v>
       </c>
       <c r="E37" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F37">
         <v>5022</v>
       </c>
       <c r="G37" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H37" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I37" t="s">
+        <v>462</v>
+      </c>
+      <c r="J37" t="s">
         <v>463</v>
-      </c>
-      <c r="J37" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>309</v>
+      </c>
+      <c r="B38" t="s">
         <v>310</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>311</v>
-      </c>
-      <c r="C38" t="s">
-        <v>312</v>
       </c>
       <c r="D38" t="s">
         <v>17</v>
       </c>
       <c r="E38" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F38">
         <v>97827</v>
       </c>
       <c r="G38" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H38" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I38" t="s">
+        <v>464</v>
+      </c>
+      <c r="J38" t="s">
         <v>465</v>
-      </c>
-      <c r="J38" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>313</v>
+      </c>
+      <c r="B39" t="s">
         <v>314</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>315</v>
-      </c>
-      <c r="C39" t="s">
-        <v>316</v>
       </c>
       <c r="D39" t="s">
         <v>9</v>
       </c>
       <c r="E39" t="s">
+        <v>466</v>
+      </c>
+      <c r="G39" t="s">
+        <v>316</v>
+      </c>
+      <c r="H39" t="s">
+        <v>317</v>
+      </c>
+      <c r="I39" t="s">
         <v>467</v>
       </c>
-      <c r="G39" t="s">
-        <v>317</v>
-      </c>
-      <c r="H39" t="s">
-        <v>318</v>
-      </c>
-      <c r="I39" t="s">
+      <c r="J39" t="s">
         <v>468</v>
-      </c>
-      <c r="J39" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>318</v>
+      </c>
+      <c r="B40" t="s">
         <v>319</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>320</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
+        <v>117</v>
+      </c>
+      <c r="E40" t="s">
+        <v>469</v>
+      </c>
+      <c r="F40" t="s">
+        <v>470</v>
+      </c>
+      <c r="G40" t="s">
+        <v>164</v>
+      </c>
+      <c r="H40" t="s">
         <v>321</v>
       </c>
-      <c r="D40" t="s">
-        <v>118</v>
-      </c>
-      <c r="E40" t="s">
-        <v>470</v>
-      </c>
-      <c r="F40" t="s">
+      <c r="I40" t="s">
         <v>471</v>
-      </c>
-      <c r="G40" t="s">
-        <v>165</v>
-      </c>
-      <c r="H40" t="s">
-        <v>322</v>
-      </c>
-      <c r="I40" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>322</v>
+      </c>
+      <c r="B41" t="s">
         <v>323</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>324</v>
-      </c>
-      <c r="C41" t="s">
-        <v>325</v>
       </c>
       <c r="D41" t="s">
         <v>9</v>
@@ -3331,24 +3337,24 @@
         <v>14776</v>
       </c>
       <c r="G41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H41" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I41" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>326</v>
+      </c>
+      <c r="B42" t="s">
         <v>327</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>328</v>
-      </c>
-      <c r="C42" t="s">
-        <v>329</v>
       </c>
       <c r="D42" t="s">
         <v>17</v>
@@ -3357,120 +3363,120 @@
         <v>78000</v>
       </c>
       <c r="G42" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H42" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I42" t="s">
+        <v>473</v>
+      </c>
+      <c r="J42" t="s">
         <v>474</v>
-      </c>
-      <c r="J42" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>330</v>
+      </c>
+      <c r="B43" t="s">
         <v>331</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>332</v>
       </c>
-      <c r="C43" t="s">
-        <v>333</v>
-      </c>
       <c r="D43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F43">
         <v>31000</v>
       </c>
       <c r="G43" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I43" t="s">
+        <v>475</v>
+      </c>
+      <c r="J43" t="s">
         <v>476</v>
-      </c>
-      <c r="J43" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>334</v>
+      </c>
+      <c r="B44" t="s">
         <v>335</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>336</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
+        <v>56</v>
+      </c>
+      <c r="E44" t="s">
+        <v>135</v>
+      </c>
+      <c r="F44" t="s">
+        <v>477</v>
+      </c>
+      <c r="G44" t="s">
+        <v>171</v>
+      </c>
+      <c r="H44" t="s">
         <v>337</v>
       </c>
-      <c r="D44" t="s">
-        <v>57</v>
-      </c>
-      <c r="E44" t="s">
-        <v>136</v>
-      </c>
-      <c r="F44" t="s">
+      <c r="I44" t="s">
         <v>478</v>
       </c>
-      <c r="G44" t="s">
-        <v>172</v>
-      </c>
-      <c r="H44" t="s">
-        <v>338</v>
-      </c>
-      <c r="I44" t="s">
+      <c r="J44" t="s">
         <v>479</v>
-      </c>
-      <c r="J44" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>338</v>
+      </c>
+      <c r="B45" t="s">
         <v>339</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>340</v>
       </c>
-      <c r="C45" t="s">
-        <v>341</v>
-      </c>
       <c r="D45" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E45" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F45">
         <v>99362</v>
       </c>
       <c r="G45" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H45" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="I45" t="s">
+        <v>481</v>
+      </c>
+      <c r="J45" t="s">
         <v>482</v>
-      </c>
-      <c r="J45" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>342</v>
+      </c>
+      <c r="B46" t="s">
         <v>343</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>344</v>
-      </c>
-      <c r="C46" t="s">
-        <v>345</v>
       </c>
       <c r="D46" t="s">
         <v>17</v>
@@ -3479,358 +3485,358 @@
         <v>60528</v>
       </c>
       <c r="G46" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H46" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I46" t="s">
+        <v>483</v>
+      </c>
+      <c r="J46" t="s">
         <v>484</v>
-      </c>
-      <c r="J46" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>346</v>
+      </c>
+      <c r="B47" t="s">
         <v>347</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>348</v>
-      </c>
-      <c r="C47" t="s">
-        <v>349</v>
       </c>
       <c r="D47" t="s">
         <v>3</v>
       </c>
       <c r="E47" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F47">
         <v>94117</v>
       </c>
       <c r="G47" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H47" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="I47" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>350</v>
+      </c>
+      <c r="B48" t="s">
         <v>351</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>352</v>
       </c>
-      <c r="C48" t="s">
-        <v>353</v>
-      </c>
       <c r="D48" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E48" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F48">
         <v>3508</v>
       </c>
       <c r="G48" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H48" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I48" t="s">
+        <v>488</v>
+      </c>
+      <c r="J48" t="s">
         <v>489</v>
-      </c>
-      <c r="J48" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>354</v>
+      </c>
+      <c r="B49" t="s">
         <v>355</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>356</v>
-      </c>
-      <c r="C49" t="s">
-        <v>357</v>
       </c>
       <c r="D49" t="s">
         <v>3</v>
       </c>
       <c r="E49" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F49">
         <v>4980</v>
       </c>
       <c r="G49" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H49" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="I49" t="s">
+        <v>491</v>
+      </c>
+      <c r="J49" t="s">
         <v>492</v>
-      </c>
-      <c r="J49" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>358</v>
+      </c>
+      <c r="B50" t="s">
         <v>359</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>360</v>
       </c>
-      <c r="C50" t="s">
-        <v>361</v>
-      </c>
       <c r="D50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E50" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F50">
         <v>97219</v>
       </c>
       <c r="G50" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H50" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I50" t="s">
+        <v>493</v>
+      </c>
+      <c r="J50" t="s">
         <v>494</v>
-      </c>
-      <c r="J50" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>361</v>
+      </c>
+      <c r="B51" t="s">
         <v>362</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>363</v>
       </c>
-      <c r="C51" t="s">
-        <v>364</v>
-      </c>
       <c r="D51" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F51">
         <v>24100</v>
       </c>
       <c r="G51" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H51" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I51" t="s">
+        <v>495</v>
+      </c>
+      <c r="J51" t="s">
         <v>496</v>
-      </c>
-      <c r="J51" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>365</v>
+      </c>
+      <c r="B52" t="s">
         <v>366</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>367</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
+        <v>42</v>
+      </c>
+      <c r="F52" t="s">
+        <v>497</v>
+      </c>
+      <c r="G52" t="s">
+        <v>204</v>
+      </c>
+      <c r="H52" t="s">
         <v>368</v>
       </c>
-      <c r="D52" t="s">
-        <v>43</v>
-      </c>
-      <c r="F52" t="s">
+      <c r="I52" t="s">
         <v>498</v>
       </c>
-      <c r="G52" t="s">
-        <v>205</v>
-      </c>
-      <c r="H52" t="s">
-        <v>369</v>
-      </c>
-      <c r="I52" t="s">
+      <c r="J52" t="s">
         <v>499</v>
-      </c>
-      <c r="J52" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>369</v>
+      </c>
+      <c r="B53" t="s">
         <v>370</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
         <v>371</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
+        <v>56</v>
+      </c>
+      <c r="E53" t="s">
+        <v>500</v>
+      </c>
+      <c r="F53" t="s">
+        <v>501</v>
+      </c>
+      <c r="G53" t="s">
+        <v>171</v>
+      </c>
+      <c r="H53" t="s">
         <v>372</v>
       </c>
-      <c r="D53" t="s">
-        <v>57</v>
-      </c>
-      <c r="E53" t="s">
-        <v>501</v>
-      </c>
-      <c r="F53" t="s">
+      <c r="I53" t="s">
         <v>502</v>
       </c>
-      <c r="G53" t="s">
-        <v>172</v>
-      </c>
-      <c r="H53" t="s">
-        <v>373</v>
-      </c>
-      <c r="I53" t="s">
+      <c r="J53" t="s">
         <v>503</v>
-      </c>
-      <c r="J53" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
+        <v>373</v>
+      </c>
+      <c r="B54" t="s">
         <v>374</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>375</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
+        <v>56</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="G54" t="s">
+        <v>162</v>
+      </c>
+      <c r="H54" t="s">
         <v>376</v>
       </c>
-      <c r="D54" t="s">
-        <v>57</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>588</v>
-      </c>
-      <c r="G54" t="s">
-        <v>163</v>
-      </c>
-      <c r="H54" t="s">
-        <v>377</v>
-      </c>
       <c r="I54" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>377</v>
+      </c>
+      <c r="B55" t="s">
         <v>378</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>379</v>
-      </c>
-      <c r="C55" t="s">
-        <v>380</v>
       </c>
       <c r="D55" t="s">
         <v>9</v>
       </c>
       <c r="F55" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G55" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H55" t="s">
         <v>19</v>
       </c>
       <c r="I55" t="s">
+        <v>506</v>
+      </c>
+      <c r="J55" t="s">
         <v>507</v>
-      </c>
-      <c r="J55" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>380</v>
+      </c>
+      <c r="B56" t="s">
         <v>381</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
         <v>382</v>
       </c>
-      <c r="C56" t="s">
-        <v>383</v>
-      </c>
       <c r="D56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F56">
         <v>1010</v>
       </c>
       <c r="G56" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H56" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I56" t="s">
+        <v>508</v>
+      </c>
+      <c r="J56" t="s">
         <v>509</v>
-      </c>
-      <c r="J56" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>383</v>
+      </c>
+      <c r="B57" t="s">
         <v>384</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
         <v>385</v>
-      </c>
-      <c r="C57" t="s">
-        <v>386</v>
       </c>
       <c r="D57" t="s">
         <v>17</v>
       </c>
       <c r="E57" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F57">
         <v>99508</v>
       </c>
       <c r="G57" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H57" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I57" t="s">
+        <v>511</v>
+      </c>
+      <c r="J57" t="s">
         <v>512</v>
-      </c>
-      <c r="J57" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
+        <v>387</v>
+      </c>
+      <c r="B58" t="s">
         <v>388</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
         <v>389</v>
-      </c>
-      <c r="C58" t="s">
-        <v>390</v>
       </c>
       <c r="D58" t="s">
         <v>3</v>
@@ -3839,27 +3845,27 @@
         <v>50739</v>
       </c>
       <c r="G58" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H58" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I58" t="s">
+        <v>513</v>
+      </c>
+      <c r="J58" t="s">
         <v>514</v>
-      </c>
-      <c r="J58" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
+        <v>391</v>
+      </c>
+      <c r="B59" t="s">
         <v>392</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
         <v>393</v>
-      </c>
-      <c r="C59" t="s">
-        <v>394</v>
       </c>
       <c r="D59" t="s">
         <v>3</v>
@@ -3868,85 +3874,85 @@
         <v>75012</v>
       </c>
       <c r="G59" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H59" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I59" t="s">
+        <v>515</v>
+      </c>
+      <c r="J59" t="s">
         <v>516</v>
-      </c>
-      <c r="J59" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
+        <v>394</v>
+      </c>
+      <c r="B60" t="s">
         <v>395</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" t="s">
         <v>396</v>
-      </c>
-      <c r="C60" t="s">
-        <v>397</v>
       </c>
       <c r="D60" t="s">
         <v>17</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="G60" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I60" t="s">
+        <v>517</v>
+      </c>
+      <c r="J60" t="s">
         <v>518</v>
-      </c>
-      <c r="J60" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
+        <v>397</v>
+      </c>
+      <c r="B61" t="s">
         <v>398</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
         <v>399</v>
       </c>
-      <c r="C61" t="s">
-        <v>400</v>
-      </c>
       <c r="D61" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F61">
         <v>5020</v>
       </c>
       <c r="G61" t="s">
+        <v>400</v>
+      </c>
+      <c r="H61" t="s">
         <v>401</v>
       </c>
-      <c r="H61" t="s">
-        <v>402</v>
-      </c>
       <c r="I61" t="s">
+        <v>519</v>
+      </c>
+      <c r="J61" t="s">
         <v>520</v>
-      </c>
-      <c r="J61" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>402</v>
+      </c>
+      <c r="B62" t="s">
         <v>403</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
         <v>404</v>
-      </c>
-      <c r="C62" t="s">
-        <v>405</v>
       </c>
       <c r="D62" t="s">
         <v>17</v>
@@ -3955,111 +3961,111 @@
         <v>1756</v>
       </c>
       <c r="G62" t="s">
+        <v>278</v>
+      </c>
+      <c r="H62" t="s">
         <v>279</v>
       </c>
-      <c r="H62" t="s">
-        <v>280</v>
-      </c>
       <c r="I62" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
+        <v>405</v>
+      </c>
+      <c r="B63" t="s">
         <v>406</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" t="s">
         <v>407</v>
       </c>
-      <c r="C63" t="s">
-        <v>408</v>
-      </c>
       <c r="D63" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E63" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F63" t="s">
+        <v>522</v>
+      </c>
+      <c r="G63" t="s">
+        <v>170</v>
+      </c>
+      <c r="H63" t="s">
+        <v>304</v>
+      </c>
+      <c r="I63" t="s">
         <v>523</v>
       </c>
-      <c r="G63" t="s">
-        <v>171</v>
-      </c>
-      <c r="H63" t="s">
-        <v>305</v>
-      </c>
-      <c r="I63" t="s">
+      <c r="J63" t="s">
         <v>524</v>
-      </c>
-      <c r="J63" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
+        <v>408</v>
+      </c>
+      <c r="B64" t="s">
         <v>409</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
         <v>410</v>
       </c>
-      <c r="C64" t="s">
-        <v>411</v>
-      </c>
       <c r="D64" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E64" t="s">
         <v>10</v>
       </c>
       <c r="F64" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="G64" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H64" t="s">
         <v>12</v>
       </c>
       <c r="I64" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
+        <v>411</v>
+      </c>
+      <c r="B65" t="s">
         <v>412</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
         <v>413</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
+        <v>62</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="G65" t="s">
+        <v>162</v>
+      </c>
+      <c r="H65" t="s">
         <v>414</v>
       </c>
-      <c r="D65" t="s">
-        <v>63</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>590</v>
-      </c>
-      <c r="G65" t="s">
-        <v>163</v>
-      </c>
-      <c r="H65" t="s">
-        <v>415</v>
-      </c>
       <c r="I65" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
+        <v>415</v>
+      </c>
+      <c r="B66" t="s">
         <v>416</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
         <v>417</v>
-      </c>
-      <c r="C66" t="s">
-        <v>418</v>
       </c>
       <c r="D66" t="s">
         <v>17</v>
@@ -4068,59 +4074,59 @@
         <v>1010</v>
       </c>
       <c r="G66" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H66" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I66" t="s">
+        <v>528</v>
+      </c>
+      <c r="J66" t="s">
         <v>529</v>
-      </c>
-      <c r="J66" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
+        <v>418</v>
+      </c>
+      <c r="B67" t="s">
         <v>419</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
         <v>420</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>421</v>
       </c>
-      <c r="D67" t="s">
-        <v>422</v>
-      </c>
       <c r="E67" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F67">
         <v>87110</v>
       </c>
       <c r="G67" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H67" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="I67" t="s">
+        <v>531</v>
+      </c>
+      <c r="J67" t="s">
         <v>532</v>
-      </c>
-      <c r="J67" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>423</v>
+      </c>
+      <c r="B68" t="s">
         <v>424</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
         <v>425</v>
-      </c>
-      <c r="C68" t="s">
-        <v>426</v>
       </c>
       <c r="D68" t="s">
         <v>9</v>
@@ -4129,111 +4135,111 @@
         <v>42100</v>
       </c>
       <c r="G68" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H68" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="I68" t="s">
+        <v>533</v>
+      </c>
+      <c r="J68" t="s">
         <v>534</v>
-      </c>
-      <c r="J68" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
+        <v>427</v>
+      </c>
+      <c r="B69" t="s">
         <v>428</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
         <v>429</v>
       </c>
-      <c r="C69" t="s">
-        <v>430</v>
-      </c>
       <c r="D69" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E69" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F69" t="s">
+        <v>535</v>
+      </c>
+      <c r="G69" t="s">
+        <v>170</v>
+      </c>
+      <c r="H69" t="s">
+        <v>304</v>
+      </c>
+      <c r="I69" t="s">
         <v>536</v>
-      </c>
-      <c r="G69" t="s">
-        <v>171</v>
-      </c>
-      <c r="H69" t="s">
-        <v>305</v>
-      </c>
-      <c r="I69" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
+        <v>430</v>
+      </c>
+      <c r="B70" t="s">
         <v>431</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
         <v>432</v>
       </c>
-      <c r="C70" t="s">
-        <v>433</v>
-      </c>
       <c r="D70" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F70">
         <v>1203</v>
       </c>
       <c r="G70" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H70" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="I70" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
+        <v>172</v>
+      </c>
+      <c r="B71" t="s">
         <v>173</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" t="s">
         <v>174</v>
       </c>
-      <c r="C71" t="s">
-        <v>175</v>
-      </c>
       <c r="D71" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F71">
         <v>28001</v>
       </c>
       <c r="G71" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H71" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I71" t="s">
+        <v>538</v>
+      </c>
+      <c r="J71" t="s">
         <v>539</v>
-      </c>
-      <c r="J71" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
+        <v>175</v>
+      </c>
+      <c r="B72" t="s">
         <v>176</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" t="s">
         <v>177</v>
-      </c>
-      <c r="C72" t="s">
-        <v>178</v>
       </c>
       <c r="D72" t="s">
         <v>3</v>
@@ -4242,85 +4248,85 @@
         <v>4110</v>
       </c>
       <c r="G72" t="s">
+        <v>178</v>
+      </c>
+      <c r="H72" t="s">
         <v>179</v>
       </c>
-      <c r="H72" t="s">
-        <v>180</v>
-      </c>
       <c r="I72" t="s">
+        <v>540</v>
+      </c>
+      <c r="J72" t="s">
         <v>541</v>
-      </c>
-      <c r="J72" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
+        <v>180</v>
+      </c>
+      <c r="B73" t="s">
         <v>181</v>
       </c>
-      <c r="B73" t="s">
+      <c r="C73" t="s">
         <v>182</v>
-      </c>
-      <c r="C73" t="s">
-        <v>183</v>
       </c>
       <c r="D73" t="s">
         <v>17</v>
       </c>
       <c r="E73" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F73">
         <v>83720</v>
       </c>
       <c r="G73" t="s">
+        <v>183</v>
+      </c>
+      <c r="H73" t="s">
         <v>184</v>
       </c>
-      <c r="H73" t="s">
-        <v>185</v>
-      </c>
       <c r="I73" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
+        <v>185</v>
+      </c>
+      <c r="B74" t="s">
         <v>186</v>
       </c>
-      <c r="B74" t="s">
+      <c r="C74" t="s">
         <v>187</v>
       </c>
-      <c r="C74" t="s">
-        <v>188</v>
-      </c>
       <c r="D74" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F74" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="G74" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H74" t="s">
         <v>19</v>
       </c>
       <c r="I74" t="s">
+        <v>544</v>
+      </c>
+      <c r="J74" t="s">
         <v>545</v>
-      </c>
-      <c r="J74" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
+        <v>188</v>
+      </c>
+      <c r="B75" t="s">
         <v>189</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" t="s">
         <v>190</v>
-      </c>
-      <c r="C75" t="s">
-        <v>191</v>
       </c>
       <c r="D75" t="s">
         <v>3</v>
@@ -4329,233 +4335,233 @@
         <v>1734</v>
       </c>
       <c r="G75" t="s">
+        <v>191</v>
+      </c>
+      <c r="H75" t="s">
         <v>192</v>
       </c>
-      <c r="H75" t="s">
-        <v>193</v>
-      </c>
       <c r="I75" t="s">
+        <v>546</v>
+      </c>
+      <c r="J75" t="s">
         <v>547</v>
-      </c>
-      <c r="J75" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
+        <v>193</v>
+      </c>
+      <c r="B76" t="s">
         <v>194</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C76" t="s">
         <v>195</v>
       </c>
-      <c r="C76" t="s">
-        <v>196</v>
-      </c>
       <c r="D76" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F76">
         <v>75016</v>
       </c>
       <c r="G76" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H76" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I76" t="s">
+        <v>548</v>
+      </c>
+      <c r="J76" t="s">
         <v>549</v>
-      </c>
-      <c r="J76" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
+        <v>197</v>
+      </c>
+      <c r="B77" t="s">
         <v>198</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C77" t="s">
         <v>199</v>
       </c>
-      <c r="C77" t="s">
-        <v>200</v>
-      </c>
       <c r="D77" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E77" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F77">
         <v>82520</v>
       </c>
       <c r="G77" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H77" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I77" t="s">
+        <v>551</v>
+      </c>
+      <c r="J77" t="s">
         <v>552</v>
-      </c>
-      <c r="J77" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
+        <v>201</v>
+      </c>
+      <c r="B78" t="s">
         <v>202</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C78" t="s">
         <v>203</v>
       </c>
-      <c r="C78" t="s">
+      <c r="D78" t="s">
+        <v>62</v>
+      </c>
+      <c r="F78" t="s">
+        <v>553</v>
+      </c>
+      <c r="G78" t="s">
         <v>204</v>
       </c>
-      <c r="D78" t="s">
-        <v>63</v>
-      </c>
-      <c r="F78" t="s">
+      <c r="H78" t="s">
+        <v>205</v>
+      </c>
+      <c r="I78" t="s">
         <v>554</v>
       </c>
-      <c r="G78" t="s">
-        <v>205</v>
-      </c>
-      <c r="H78" t="s">
-        <v>206</v>
-      </c>
-      <c r="I78" t="s">
+      <c r="J78" t="s">
         <v>555</v>
-      </c>
-      <c r="J78" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
+        <v>206</v>
+      </c>
+      <c r="B79" t="s">
         <v>207</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C79" t="s">
         <v>208</v>
       </c>
-      <c r="C79" t="s">
-        <v>209</v>
-      </c>
       <c r="D79" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E79" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F79">
         <v>97201</v>
       </c>
       <c r="G79" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H79" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I79" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
+        <v>210</v>
+      </c>
+      <c r="B80" t="s">
         <v>211</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C80" t="s">
         <v>212</v>
       </c>
-      <c r="C80" t="s">
-        <v>213</v>
-      </c>
       <c r="D80" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E80" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F80">
         <v>59801</v>
       </c>
       <c r="G80" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H80" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I80" t="s">
+        <v>558</v>
+      </c>
+      <c r="J80" t="s">
         <v>559</v>
-      </c>
-      <c r="J80" t="s">
-        <v>560</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
+        <v>214</v>
+      </c>
+      <c r="B81" t="s">
         <v>215</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" t="s">
         <v>216</v>
       </c>
-      <c r="C81" t="s">
-        <v>217</v>
-      </c>
       <c r="D81" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F81">
         <v>44087</v>
       </c>
       <c r="G81" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H81" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I81" t="s">
+        <v>560</v>
+      </c>
+      <c r="J81" t="s">
         <v>561</v>
-      </c>
-      <c r="J81" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
+        <v>218</v>
+      </c>
+      <c r="B82" t="s">
         <v>219</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" t="s">
         <v>220</v>
-      </c>
-      <c r="C82" t="s">
-        <v>221</v>
       </c>
       <c r="D82" t="s">
         <v>3</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="G82" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H82" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I82" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
+        <v>221</v>
+      </c>
+      <c r="B83" t="s">
         <v>222</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" t="s">
         <v>223</v>
-      </c>
-      <c r="C83" t="s">
-        <v>224</v>
       </c>
       <c r="D83" t="s">
         <v>17</v>
@@ -4564,286 +4570,286 @@
         <v>10</v>
       </c>
       <c r="F83" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G83" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H83" t="s">
         <v>12</v>
       </c>
       <c r="I83" t="s">
+        <v>564</v>
+      </c>
+      <c r="J83" t="s">
         <v>565</v>
-      </c>
-      <c r="J83" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
+        <v>224</v>
+      </c>
+      <c r="B84" t="s">
         <v>225</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C84" t="s">
         <v>226</v>
-      </c>
-      <c r="C84" t="s">
-        <v>227</v>
       </c>
       <c r="D84" t="s">
         <v>9</v>
       </c>
       <c r="E84" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F84">
         <v>98034</v>
       </c>
       <c r="G84" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H84" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I84" t="s">
+        <v>566</v>
+      </c>
+      <c r="J84" t="s">
         <v>567</v>
-      </c>
-      <c r="J84" t="s">
-        <v>568</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
+        <v>228</v>
+      </c>
+      <c r="B85" t="s">
         <v>229</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85" t="s">
         <v>230</v>
       </c>
-      <c r="C85" t="s">
-        <v>231</v>
-      </c>
       <c r="D85" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F85">
         <v>8200</v>
       </c>
       <c r="G85" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H85" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I85" t="s">
+        <v>568</v>
+      </c>
+      <c r="J85" t="s">
         <v>569</v>
-      </c>
-      <c r="J85" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
+        <v>232</v>
+      </c>
+      <c r="B86" t="s">
         <v>233</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" t="s">
         <v>234</v>
       </c>
-      <c r="C86" t="s">
-        <v>235</v>
-      </c>
       <c r="D86" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F86">
         <v>69004</v>
       </c>
       <c r="G86" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H86" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I86" t="s">
+        <v>570</v>
+      </c>
+      <c r="J86" t="s">
         <v>571</v>
-      </c>
-      <c r="J86" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
+        <v>236</v>
+      </c>
+      <c r="B87" t="s">
         <v>237</v>
       </c>
-      <c r="B87" t="s">
+      <c r="C87" t="s">
         <v>238</v>
       </c>
-      <c r="C87" t="s">
-        <v>239</v>
-      </c>
       <c r="D87" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F87">
         <v>51100</v>
       </c>
       <c r="G87" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H87" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I87" t="s">
+        <v>572</v>
+      </c>
+      <c r="J87" t="s">
         <v>573</v>
-      </c>
-      <c r="J87" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
+        <v>240</v>
+      </c>
+      <c r="B88" t="s">
         <v>241</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" t="s">
         <v>242</v>
       </c>
-      <c r="C88" t="s">
-        <v>243</v>
-      </c>
       <c r="D88" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F88">
         <v>90110</v>
       </c>
       <c r="G88" t="s">
+        <v>243</v>
+      </c>
+      <c r="H88" t="s">
         <v>244</v>
       </c>
-      <c r="H88" t="s">
-        <v>245</v>
-      </c>
       <c r="I88" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="J88" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
+        <v>245</v>
+      </c>
+      <c r="B89" t="s">
         <v>246</v>
       </c>
-      <c r="B89" t="s">
+      <c r="C89" t="s">
         <v>247</v>
       </c>
-      <c r="C89" t="s">
-        <v>248</v>
-      </c>
       <c r="D89" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E89" t="s">
         <v>10</v>
       </c>
       <c r="F89" t="s">
+        <v>575</v>
+      </c>
+      <c r="G89" t="s">
+        <v>170</v>
+      </c>
+      <c r="H89" t="s">
+        <v>248</v>
+      </c>
+      <c r="I89" t="s">
         <v>576</v>
-      </c>
-      <c r="G89" t="s">
-        <v>171</v>
-      </c>
-      <c r="H89" t="s">
-        <v>249</v>
-      </c>
-      <c r="I89" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
+        <v>249</v>
+      </c>
+      <c r="B90" t="s">
         <v>250</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" t="s">
         <v>251</v>
-      </c>
-      <c r="C90" t="s">
-        <v>252</v>
       </c>
       <c r="D90" t="s">
         <v>3</v>
       </c>
       <c r="E90" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F90">
         <v>98128</v>
       </c>
       <c r="G90" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H90" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I90" t="s">
+        <v>577</v>
+      </c>
+      <c r="J90" t="s">
         <v>578</v>
-      </c>
-      <c r="J90" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
+        <v>253</v>
+      </c>
+      <c r="B91" t="s">
         <v>254</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91" t="s">
         <v>255</v>
       </c>
-      <c r="C91" t="s">
+      <c r="D91" t="s">
         <v>256</v>
-      </c>
-      <c r="D91" t="s">
-        <v>257</v>
       </c>
       <c r="F91">
         <v>21240</v>
       </c>
       <c r="G91" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H91" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I91" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="J91" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
+        <v>258</v>
+      </c>
+      <c r="B92" t="s">
         <v>259</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" t="s">
         <v>260</v>
-      </c>
-      <c r="C92" t="s">
-        <v>261</v>
       </c>
       <c r="D92" t="s">
         <v>3</v>
       </c>
       <c r="F92" t="s">
+        <v>580</v>
+      </c>
+      <c r="G92" t="s">
+        <v>261</v>
+      </c>
+      <c r="H92" t="s">
+        <v>262</v>
+      </c>
+      <c r="I92" t="s">
         <v>581</v>
       </c>
-      <c r="G92" t="s">
-        <v>262</v>
-      </c>
-      <c r="H92" t="s">
-        <v>263</v>
-      </c>
-      <c r="I92" t="s">
-        <v>582</v>
-      </c>
       <c r="J92" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
   </sheetData>

</xml_diff>